<commit_message>
tweaked gini logit & factored out gini decrease
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivercairns/Desktop/code/WeightOfEvidenceDemo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF808C5-19AB-5E48-8956-8F184A49E64D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0750E92-41B3-8F44-9728-2C746EF25FFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16120" activeTab="4" xr2:uid="{762E3304-FB65-904E-81F4-911B3579DB61}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16120" activeTab="2" xr2:uid="{762E3304-FB65-904E-81F4-911B3579DB61}"/>
   </bookViews>
   <sheets>
     <sheet name="single_var_decision_tree" sheetId="1" r:id="rId1"/>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB5FEDC-BD8C-104F-AC7C-B5B7693E67BB}">
   <dimension ref="B2:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,32 +655,32 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F3">
-        <f>COUNT(C3:$C$3)</f>
-        <v>1</v>
+        <f>COUNT(C3:$C$3)-1</f>
+        <v>0</v>
       </c>
       <c r="G3">
         <f>COUNT($C$3:$C$14)-F3</f>
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <f>SUM($C$3:C3)/F3</f>
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C3))/(G3)</f>
-        <v>0.63636363636363635</v>
-      </c>
-      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="H3" t="e">
+        <f>(SUM($C$3:C3)-C3)/F3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I3" t="e">
+        <f>(SUM($C$3:$C$14)-(H3*F3)/(G3))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" t="e">
         <f>1-(H3*H3)-((1-H3)*(1-H3))</f>
-        <v>0</v>
-      </c>
-      <c r="K3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" t="e">
         <f>1-(I3*I3)-((1-I3)*(1-I3))</f>
-        <v>0.46280991735537191</v>
-      </c>
-      <c r="L3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L3" t="e">
         <f>((F3*J3)+(G3*K3))/COUNT($C$3:$C$14)</f>
-        <v>0.42424242424242425</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="M3" t="b">
         <f>NOT(B3=B2)</f>
@@ -703,32 +703,32 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F4">
-        <f>COUNT(C$3:$C4)</f>
-        <v>2</v>
+        <f>COUNT(C$3:$C4)-1</f>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G14" si="2">COUNT($C$3:$C$14)-F4</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H4">
-        <f>SUM($C$3:C4)/F4</f>
-        <v>0.5</v>
+        <f>(SUM($C$3:C4)-C4)/F4</f>
+        <v>0</v>
       </c>
       <c r="I4">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C4))/(G4)</f>
-        <v>0.6</v>
+        <f>(SUM($C$3:$C$14)-(H4*F4))/(G4)</f>
+        <v>0.63636363636363635</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:K14" si="3">1-(H4*H4)-((1-H4)*(1-H4))</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <f t="shared" si="3"/>
-        <v>0.48</v>
+        <v>0.46280991735537191</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L14" si="4">((F4*J4)+(G4*K4))/COUNT($C$3:$C$14)</f>
-        <v>0.48333333333333334</v>
+        <v>0.42424242424242425</v>
       </c>
       <c r="M4" t="b">
         <f t="shared" ref="M4:M14" si="5">NOT(B4=B3)</f>
@@ -751,32 +751,32 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F5">
-        <f>COUNT(C$3:$C5)</f>
-        <v>3</v>
+        <f>COUNT(C$3:$C5)-1</f>
+        <v>2</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <f>SUM($C$3:C5)/F5</f>
-        <v>0.33333333333333331</v>
+        <f>(SUM($C$3:C5)-C5)/F5</f>
+        <v>0.5</v>
       </c>
       <c r="I5">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C5))/(G5)</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" ref="I5:I14" si="6">(SUM($C$3:$C$14)-(H5*F5))/(G5)</f>
+        <v>0.6</v>
       </c>
       <c r="J5">
         <f t="shared" si="3"/>
-        <v>0.44444444444444431</v>
+        <v>0.5</v>
       </c>
       <c r="K5">
         <f t="shared" si="3"/>
-        <v>0.44444444444444442</v>
+        <v>0.48</v>
       </c>
       <c r="L5">
         <f t="shared" si="4"/>
-        <v>0.44444444444444442</v>
+        <v>0.48333333333333334</v>
       </c>
       <c r="M5" t="b">
         <f t="shared" si="5"/>
@@ -799,32 +799,32 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F6">
-        <f>COUNT(C$3:$C6)</f>
-        <v>4</v>
+        <f>COUNT(C$3:$C6)-1</f>
+        <v>3</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H6">
-        <f>SUM($C$3:C6)/F6</f>
-        <v>0.25</v>
+        <f>(SUM($C$3:C6)-C6)/F6</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I6">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C6))/(G6)</f>
-        <v>0.75</v>
+        <f t="shared" si="6"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J6">
         <f t="shared" si="3"/>
-        <v>0.375</v>
+        <v>0.44444444444444431</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>0.375</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="L6">
         <f t="shared" si="4"/>
-        <v>0.375</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="M6" t="b">
         <f t="shared" si="5"/>
@@ -847,32 +847,32 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F7">
-        <f>COUNT(C$3:$C7)</f>
-        <v>5</v>
+        <f>COUNT(C$3:$C7)-1</f>
+        <v>4</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H7">
-        <f>SUM($C$3:C7)/F7</f>
-        <v>0.2</v>
+        <f>(SUM($C$3:C7)-C7)/F7</f>
+        <v>0.25</v>
       </c>
       <c r="I7">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C7))/(G7)</f>
-        <v>0.8571428571428571</v>
+        <f t="shared" si="6"/>
+        <v>0.75</v>
       </c>
       <c r="J7">
         <f t="shared" si="3"/>
-        <v>0.31999999999999984</v>
+        <v>0.375</v>
       </c>
       <c r="K7">
         <f t="shared" si="3"/>
-        <v>0.24489795918367352</v>
+        <v>0.375</v>
       </c>
       <c r="L7">
         <f t="shared" si="4"/>
-        <v>0.27619047619047615</v>
+        <v>0.375</v>
       </c>
       <c r="M7" s="1" t="b">
         <f t="shared" si="5"/>
@@ -895,32 +895,32 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F8">
-        <f>COUNT(C$3:$C8)</f>
-        <v>6</v>
+        <f>COUNT(C$3:$C8)-1</f>
+        <v>5</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H8">
-        <f>SUM($C$3:C8)/F8</f>
-        <v>0.33333333333333331</v>
+        <f>(SUM($C$3:C8)-C8)/F8</f>
+        <v>0.2</v>
       </c>
       <c r="I8">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C8))/(G8)</f>
-        <v>0.83333333333333337</v>
+        <f t="shared" si="6"/>
+        <v>0.8571428571428571</v>
       </c>
       <c r="J8">
         <f t="shared" si="3"/>
-        <v>0.44444444444444431</v>
+        <v>0.31999999999999984</v>
       </c>
       <c r="K8">
         <f t="shared" si="3"/>
-        <v>0.27777777777777768</v>
+        <v>0.24489795918367352</v>
       </c>
       <c r="L8">
         <f t="shared" si="4"/>
-        <v>0.36111111111111099</v>
+        <v>0.27619047619047615</v>
       </c>
       <c r="M8" t="b">
         <f t="shared" si="5"/>
@@ -943,32 +943,32 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F9">
-        <f>COUNT(C$3:$C9)</f>
-        <v>7</v>
+        <f>COUNT(C$3:$C9)-1</f>
+        <v>6</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H9">
-        <f>SUM($C$3:C9)/F9</f>
-        <v>0.42857142857142855</v>
+        <f>(SUM($C$3:C9)-C9)/F9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I9">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C9))/(G9)</f>
-        <v>0.8</v>
+        <f t="shared" si="6"/>
+        <v>0.83333333333333337</v>
       </c>
       <c r="J9">
         <f t="shared" si="3"/>
-        <v>0.48979591836734698</v>
+        <v>0.44444444444444431</v>
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
-        <v>0.3199999999999999</v>
+        <v>0.27777777777777768</v>
       </c>
       <c r="L9">
         <f t="shared" si="4"/>
-        <v>0.41904761904761906</v>
+        <v>0.36111111111111099</v>
       </c>
       <c r="M9" t="b">
         <f t="shared" si="5"/>
@@ -991,32 +991,32 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F10">
-        <f>COUNT(C$3:$C10)</f>
-        <v>8</v>
+        <f>COUNT(C$3:$C10)-1</f>
+        <v>7</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H10">
-        <f>SUM($C$3:C10)/F10</f>
-        <v>0.5</v>
+        <f>(SUM($C$3:C10)-C10)/F10</f>
+        <v>0.42857142857142855</v>
       </c>
       <c r="I10">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C10))/(G10)</f>
-        <v>0.75</v>
+        <f t="shared" si="6"/>
+        <v>0.8</v>
       </c>
       <c r="J10">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.48979591836734698</v>
       </c>
       <c r="K10">
         <f t="shared" si="3"/>
-        <v>0.375</v>
+        <v>0.3199999999999999</v>
       </c>
       <c r="L10">
         <f t="shared" si="4"/>
-        <v>0.45833333333333331</v>
+        <v>0.41904761904761906</v>
       </c>
       <c r="M10" t="b">
         <f t="shared" si="5"/>
@@ -1039,32 +1039,32 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F11">
-        <f>COUNT(C$3:$C11)</f>
-        <v>9</v>
+        <f>COUNT(C$3:$C11)-1</f>
+        <v>8</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H11">
-        <f>SUM($C$3:C11)/F11</f>
-        <v>0.55555555555555558</v>
+        <f>(SUM($C$3:C11)-C11)/F11</f>
+        <v>0.5</v>
       </c>
       <c r="I11">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C11))/(G11)</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="6"/>
+        <v>0.75</v>
       </c>
       <c r="J11">
         <f t="shared" si="3"/>
-        <v>0.49382716049382713</v>
+        <v>0.5</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
-        <v>0.44444444444444442</v>
+        <v>0.375</v>
       </c>
       <c r="L11">
         <f t="shared" si="4"/>
-        <v>0.48148148148148145</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="M11" t="b">
         <f t="shared" si="5"/>
@@ -1087,32 +1087,32 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F12">
-        <f>COUNT(C$3:$C12)</f>
-        <v>10</v>
+        <f>COUNT(C$3:$C12)-1</f>
+        <v>9</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12">
-        <f>SUM($C$3:C12)/F12</f>
-        <v>0.5</v>
+        <f>(SUM($C$3:C12)-C12)/F12</f>
+        <v>0.55555555555555558</v>
       </c>
       <c r="I12">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C12))/(G12)</f>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J12">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.49382716049382713</v>
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="L12">
         <f t="shared" si="4"/>
-        <v>0.41666666666666669</v>
+        <v>0.48148148148148145</v>
       </c>
       <c r="M12" t="b">
         <f t="shared" si="5"/>
@@ -1135,24 +1135,24 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F13">
-        <f>COUNT(C$3:$C13)</f>
-        <v>11</v>
+        <f>COUNT(C$3:$C13)-1</f>
+        <v>10</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <f>SUM($C$3:C13)/F13</f>
-        <v>0.54545454545454541</v>
+        <f>(SUM($C$3:C13)-C13)/F13</f>
+        <v>0.5</v>
       </c>
       <c r="I13">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C13))/(G13)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J13">
         <f t="shared" si="3"/>
-        <v>0.49586776859504139</v>
+        <v>0.5</v>
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="L13">
         <f t="shared" si="4"/>
-        <v>0.45454545454545459</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M13" t="b">
         <f t="shared" si="5"/>
@@ -1183,32 +1183,32 @@
         <v>0.48611111111111105</v>
       </c>
       <c r="F14">
-        <f>COUNT(C$3:$C14)</f>
-        <v>12</v>
+        <f>COUNT(C$3:$C14)-1</f>
+        <v>11</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <f>SUM($C$3:C14)/F14</f>
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="I14" t="e">
-        <f>(SUM($C$3:$C$14)-SUM($C$3:C14))/(G14)</f>
-        <v>#DIV/0!</v>
+        <f>(SUM($C$3:C14)-C14)/F14</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" si="3"/>
-        <v>0.48611111111111105</v>
-      </c>
-      <c r="K14" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L14" t="e">
+        <v>0.49586776859504139</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.45454545454545459</v>
       </c>
       <c r="M14" t="b">
         <f t="shared" si="5"/>
@@ -1241,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7578C083-EECE-FA44-8831-ABBAD6B85E7A}">
   <dimension ref="B2:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,8 +1266,8 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f>VLOOKUP(B3,$B$18:$E$20,4)</f>
-        <v>0.30102999566398109</v>
+        <f>VLOOKUP(B3,$B$18:$E$20,4,FALSE)</f>
+        <v>-0.40546510810816427</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -1279,8 +1279,8 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D14" si="0">VLOOKUP(B4,$B$18:$E$20,4)</f>
-        <v>0.47712125471966244</v>
+        <f t="shared" ref="D4:D14" si="0">VLOOKUP(B4,$B$18:$E$20,4,FALSE)</f>
+        <v>1.0986122886681098</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.30102999566398109</v>
+        <v>-0.40546510810816427</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.47712125471966244</v>
+        <v>1.0986122886681098</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.30102999566398109</v>
+        <v>-0.40546510810816427</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.47712125471966244</v>
+        <v>1.0986122886681098</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.30102999566398109</v>
+        <v>0.69314718055994506</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.47712125471966244</v>
+        <v>1.0986122886681098</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
@@ -1365,7 +1365,7 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0.30102999566398109</v>
+        <v>0.69314718055994506</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
@@ -1377,7 +1377,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>0.30102999566398109</v>
+        <v>0.69314718055994506</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
@@ -1389,7 +1389,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>0.30102999566398109</v>
+        <v>-0.40546510810816427</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>0.30102999566398109</v>
+        <v>-0.40546510810816427</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -1428,8 +1428,8 @@
         <v>0.4</v>
       </c>
       <c r="E18">
-        <f>LOG(D18/(1-D18))</f>
-        <v>-0.17609125905568118</v>
+        <f>LN(D18/(1-D18))</f>
+        <v>-0.40546510810816427</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -1445,8 +1445,8 @@
         <v>0.75</v>
       </c>
       <c r="E19">
-        <f t="shared" ref="E19:E20" si="2">LOG(D19/(1-D19))</f>
-        <v>0.47712125471966244</v>
+        <f t="shared" ref="E19:E20" si="2">LN(D19/(1-D19))</f>
+        <v>1.0986122886681098</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>0.30102999566398109</v>
+        <v>0.69314718055994506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>